<commit_message>
Preparando Entrega Parte A
</commit_message>
<xml_diff>
--- a/Reporte_Gestion_Inmobiliaria.xlsx
+++ b/Reporte_Gestion_Inmobiliaria.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="116">
   <si>
     <t>Id Edificio</t>
   </si>
@@ -192,6 +192,9 @@
     <t>13</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
     <t>15</t>
   </si>
   <si>
@@ -223,9 +226,6 @@
   </si>
   <si>
     <t>21</t>
-  </si>
-  <si>
-    <t>14</t>
   </si>
   <si>
     <t>22</t>
@@ -486,7 +486,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -940,10 +940,10 @@
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
         <v>44</v>
@@ -952,10 +952,10 @@
         <v>2.0</v>
       </c>
       <c r="G17" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H17" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
       <c r="I17" t="s">
         <v>33</v>
@@ -969,25 +969,25 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F18" t="n">
         <v>2.0</v>
       </c>
       <c r="G18" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H18" t="n">
-        <v>60.0</v>
+        <v>45.0</v>
       </c>
       <c r="I18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19">
@@ -998,22 +998,22 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
         <v>51</v>
       </c>
       <c r="F19" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G19" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H19" t="n">
-        <v>36.0</v>
+        <v>60.0</v>
       </c>
       <c r="I19" t="s">
         <v>31</v>
@@ -1021,82 +1021,82 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G22" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H22" t="n">
-        <v>56.0</v>
+        <v>22</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F23" t="n">
         <v>2.0</v>
@@ -1113,19 +1113,19 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F24" t="n">
         <v>2.0</v>
@@ -1137,24 +1137,24 @@
         <v>56.0</v>
       </c>
       <c r="I24" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="F25" t="n">
         <v>2.0</v>
@@ -1171,28 +1171,28 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F26" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G26" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H26" t="n">
-        <v>36.0</v>
+        <v>56.0</v>
       </c>
       <c r="I26" t="s">
         <v>31</v>
@@ -1200,13 +1200,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1224,33 +1224,33 @@
         <v>36.0</v>
       </c>
       <c r="I27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F28" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G28" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H28" t="n">
-        <v>45.0</v>
+        <v>36.0</v>
       </c>
       <c r="I28" t="s">
         <v>33</v>
@@ -1258,19 +1258,19 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" t="s">
         <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F29" t="n">
         <v>2.0</v>
@@ -1282,21 +1282,21 @@
         <v>45.0</v>
       </c>
       <c r="I29" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
         <v>38</v>
@@ -1305,30 +1305,30 @@
         <v>2.0</v>
       </c>
       <c r="G30" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H30" t="n">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
       <c r="I30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
         <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F31" t="n">
         <v>2.0</v>
@@ -1345,16 +1345,16 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E32" t="s">
         <v>44</v>
@@ -1363,10 +1363,10 @@
         <v>2.0</v>
       </c>
       <c r="G32" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H32" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
       <c r="I32" t="s">
         <v>33</v>
@@ -1374,57 +1374,57 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F33" t="n">
         <v>2.0</v>
       </c>
       <c r="G33" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H33" t="n">
-        <v>60.0</v>
+        <v>45.0</v>
       </c>
       <c r="I33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
         <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E34" t="s">
         <v>51</v>
       </c>
       <c r="F34" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G34" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H34" t="n">
-        <v>36.0</v>
+        <v>60.0</v>
       </c>
       <c r="I34" t="s">
         <v>31</v>
@@ -1432,19 +1432,19 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
         <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F35" t="n">
         <v>1.0</v>
@@ -1461,13 +1461,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D36" t="s">
         <v>29</v>
@@ -1485,33 +1485,33 @@
         <v>36.0</v>
       </c>
       <c r="I36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E37" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F37" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G37" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H37" t="n">
-        <v>45.0</v>
+        <v>36.0</v>
       </c>
       <c r="I37" t="s">
         <v>33</v>
@@ -1519,19 +1519,19 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
         <v>35</v>
       </c>
       <c r="E38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F38" t="n">
         <v>2.0</v>
@@ -1543,21 +1543,21 @@
         <v>45.0</v>
       </c>
       <c r="I38" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E39" t="s">
         <v>38</v>
@@ -1566,30 +1566,30 @@
         <v>2.0</v>
       </c>
       <c r="G39" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H39" t="n">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
       <c r="I39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D40" t="s">
         <v>41</v>
       </c>
       <c r="E40" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F40" t="n">
         <v>2.0</v>
@@ -1606,16 +1606,16 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D41" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E41" t="s">
         <v>44</v>
@@ -1624,10 +1624,10 @@
         <v>2.0</v>
       </c>
       <c r="G41" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H41" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
       <c r="I41" t="s">
         <v>33</v>
@@ -1635,57 +1635,57 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B42" t="s">
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E42" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F42" t="n">
         <v>2.0</v>
       </c>
       <c r="G42" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H42" t="n">
-        <v>60.0</v>
+        <v>45.0</v>
       </c>
       <c r="I42" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D43" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
         <v>51</v>
       </c>
       <c r="F43" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G43" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H43" t="n">
-        <v>36.0</v>
+        <v>60.0</v>
       </c>
       <c r="I43" t="s">
         <v>31</v>
@@ -1693,82 +1693,82 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" t="s">
+        <v>51</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" t="s">
-        <v>22</v>
-      </c>
-      <c r="F45" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" t="s">
-        <v>24</v>
-      </c>
-      <c r="H45" t="s">
-        <v>25</v>
-      </c>
-      <c r="I45" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D46" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="E46" t="s">
-        <v>51</v>
-      </c>
-      <c r="F46" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H46" t="n">
-        <v>50.0</v>
+        <v>22</v>
+      </c>
+      <c r="F46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" t="s">
+        <v>24</v>
+      </c>
+      <c r="H46" t="s">
+        <v>25</v>
       </c>
       <c r="I46" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
         <v>99</v>
       </c>
       <c r="E47" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F47" t="n">
         <v>2.0</v>
@@ -1780,24 +1780,24 @@
         <v>50.0</v>
       </c>
       <c r="I47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
         <v>99</v>
       </c>
       <c r="E48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F48" t="n">
         <v>2.0</v>
@@ -1809,24 +1809,24 @@
         <v>50.0</v>
       </c>
       <c r="I48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D49" t="s">
         <v>99</v>
       </c>
       <c r="E49" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="F49" t="n">
         <v>2.0</v>
@@ -1838,24 +1838,24 @@
         <v>50.0</v>
       </c>
       <c r="I49" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="E50" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="F50" t="n">
         <v>2.0</v>
@@ -1864,27 +1864,27 @@
         <v>3.0</v>
       </c>
       <c r="H50" t="n">
-        <v>56.0</v>
+        <v>50.0</v>
       </c>
       <c r="I50" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F51" t="n">
         <v>2.0</v>
@@ -1901,19 +1901,19 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F52" t="n">
         <v>2.0</v>
@@ -1925,24 +1925,24 @@
         <v>56.0</v>
       </c>
       <c r="I52" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D53" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E53" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="F53" t="n">
         <v>2.0</v>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
@@ -1968,19 +1968,19 @@
         <v>59</v>
       </c>
       <c r="D54" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="E54" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F54" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G54" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H54" t="n">
-        <v>36.0</v>
+        <v>56.0</v>
       </c>
       <c r="I54" t="s">
         <v>31</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
@@ -2012,12 +2012,12 @@
         <v>36.0</v>
       </c>
       <c r="I55" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
@@ -2026,19 +2026,19 @@
         <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E56" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F56" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G56" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H56" t="n">
-        <v>45.0</v>
+        <v>36.0</v>
       </c>
       <c r="I56" t="s">
         <v>33</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -2058,7 +2058,7 @@
         <v>35</v>
       </c>
       <c r="E57" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F57" t="n">
         <v>2.0</v>
@@ -2070,21 +2070,21 @@
         <v>45.0</v>
       </c>
       <c r="I57" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D58" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E58" t="s">
         <v>38</v>
@@ -2093,30 +2093,30 @@
         <v>2.0</v>
       </c>
       <c r="G58" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H58" t="n">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
       <c r="I58" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
         <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D59" t="s">
         <v>41</v>
       </c>
       <c r="E59" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F59" t="n">
         <v>2.0</v>
@@ -2133,16 +2133,16 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B60" t="s">
         <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E60" t="s">
         <v>44</v>
@@ -2151,10 +2151,10 @@
         <v>2.0</v>
       </c>
       <c r="G60" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H60" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
       <c r="I60" t="s">
         <v>33</v>
@@ -2162,57 +2162,57 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B61" t="s">
         <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D61" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E61" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F61" t="n">
         <v>2.0</v>
       </c>
       <c r="G61" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H61" t="n">
-        <v>60.0</v>
+        <v>45.0</v>
       </c>
       <c r="I61" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B62" t="s">
         <v>14</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D62" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E62" t="s">
         <v>51</v>
       </c>
       <c r="F62" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G62" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H62" t="n">
-        <v>36.0</v>
+        <v>60.0</v>
       </c>
       <c r="I62" t="s">
         <v>31</v>
@@ -2220,19 +2220,19 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D63" t="s">
         <v>29</v>
       </c>
       <c r="E63" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F63" t="n">
         <v>1.0</v>
@@ -2249,13 +2249,13 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
         <v>39</v>
       </c>
       <c r="C64" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D64" t="s">
         <v>29</v>
@@ -2273,33 +2273,33 @@
         <v>36.0</v>
       </c>
       <c r="I64" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
         <v>39</v>
       </c>
       <c r="C65" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D65" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E65" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F65" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G65" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H65" t="n">
-        <v>45.0</v>
+        <v>36.0</v>
       </c>
       <c r="I65" t="s">
         <v>33</v>
@@ -2307,19 +2307,19 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B66" t="s">
         <v>39</v>
       </c>
       <c r="C66" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D66" t="s">
         <v>35</v>
       </c>
       <c r="E66" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F66" t="n">
         <v>2.0</v>
@@ -2331,21 +2331,21 @@
         <v>45.0</v>
       </c>
       <c r="I66" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B67" t="s">
         <v>39</v>
       </c>
       <c r="C67" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D67" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E67" t="s">
         <v>38</v>
@@ -2354,30 +2354,30 @@
         <v>2.0</v>
       </c>
       <c r="G67" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H67" t="n">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
       <c r="I67" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C68" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D68" t="s">
         <v>41</v>
       </c>
       <c r="E68" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F68" t="n">
         <v>2.0</v>
@@ -2394,16 +2394,16 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B69" t="s">
         <v>42</v>
       </c>
       <c r="C69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D69" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E69" t="s">
         <v>44</v>
@@ -2412,10 +2412,10 @@
         <v>2.0</v>
       </c>
       <c r="G69" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H69" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
       <c r="I69" t="s">
         <v>33</v>
@@ -2423,59 +2423,88 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B70" t="s">
         <v>42</v>
       </c>
       <c r="C70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D70" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E70" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F70" t="n">
         <v>2.0</v>
       </c>
       <c r="G70" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H70" t="n">
-        <v>60.0</v>
+        <v>45.0</v>
       </c>
       <c r="I70" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B71" t="s">
         <v>42</v>
       </c>
       <c r="C71" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D71" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E71" t="s">
         <v>51</v>
       </c>
       <c r="F71" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="I71" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" t="s">
+        <v>104</v>
+      </c>
+      <c r="D72" t="s">
+        <v>29</v>
+      </c>
+      <c r="E72" t="s">
+        <v>51</v>
+      </c>
+      <c r="F72" t="n">
         <v>1.0</v>
       </c>
-      <c r="G71" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H71" t="n">
+      <c r="G72" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H72" t="n">
         <v>36.0</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I72" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Preparando EP4, se agregaron datos, mejor modularizacion, clase abstracta
</commit_message>
<xml_diff>
--- a/Reporte_Gestion_Inmobiliaria.xlsx
+++ b/Reporte_Gestion_Inmobiliaria.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="132">
   <si>
     <t>Id Edificio</t>
   </si>
@@ -33,6 +33,45 @@
     <t>1</t>
   </si>
   <si>
+    <t>Vista parque</t>
+  </si>
+  <si>
+    <t>Los Médanos 129</t>
+  </si>
+  <si>
+    <t>Reñaca</t>
+  </si>
+  <si>
+    <t>Roberto Rau</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Bordemar</t>
+  </si>
+  <si>
+    <t>Las Perlas 2204</t>
+  </si>
+  <si>
+    <t>Loreto Isla</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Alto Jardín</t>
+  </si>
+  <si>
+    <t>av.Antofagasta 105</t>
+  </si>
+  <si>
+    <t>Ismael Loyi</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Viana Miramar</t>
   </si>
   <si>
@@ -42,10 +81,7 @@
     <t>Viña del mar</t>
   </si>
   <si>
-    <t>Roberto Rau</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>5</t>
   </si>
   <si>
     <t>LADY</t>
@@ -57,7 +93,7 @@
     <t>Mario Castañeda</t>
   </si>
   <si>
-    <t>3</t>
+    <t>6</t>
   </si>
   <si>
     <t>10 norte</t>
@@ -69,6 +105,45 @@
     <t>Quiroz y Puelma Arquitectos</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Motel Sunset</t>
+  </si>
+  <si>
+    <t>calle Bellavista 947</t>
+  </si>
+  <si>
+    <t>viña del mar</t>
+  </si>
+  <si>
+    <t>Oriel Badillo</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Motel adeux</t>
+  </si>
+  <si>
+    <t>camino internacional 380</t>
+  </si>
+  <si>
+    <t>Constanza Arancibia</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Motel Marina Suit</t>
+  </si>
+  <si>
+    <t>11 Nte.760</t>
+  </si>
+  <si>
+    <t>javier acuña</t>
+  </si>
+  <si>
     <t>Id Departamento</t>
   </si>
   <si>
@@ -132,36 +207,24 @@
     <t>NorOeste</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>210</t>
   </si>
   <si>
     <t>2400</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>220</t>
   </si>
   <si>
     <t>Oeste</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>230</t>
   </si>
   <si>
     <t>2890</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>240</t>
   </si>
   <si>
@@ -171,15 +234,9 @@
     <t>Este</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>250</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -352,15 +409,6 @@
   </si>
   <si>
     <t>62</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>65</t>
   </si>
 </sst>
 </file>
@@ -405,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -479,6 +527,108 @@
         <v>17</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -486,7 +636,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -499,48 +649,48 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="F3" t="n">
         <v>1.0</v>
@@ -552,7 +702,7 @@
         <v>36.0</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
@@ -563,13 +713,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="F4" t="n">
         <v>1.0</v>
@@ -581,7 +731,7 @@
         <v>36.0</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
@@ -592,13 +742,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="F5" t="n">
         <v>2.0</v>
@@ -610,7 +760,7 @@
         <v>45.0</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
@@ -621,13 +771,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="F6" t="n">
         <v>2.0</v>
@@ -639,24 +789,24 @@
         <v>45.0</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="F7" t="n">
         <v>2.0</v>
@@ -668,24 +818,24 @@
         <v>40.0</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="F8" t="n">
         <v>2.0</v>
@@ -697,24 +847,24 @@
         <v>40.0</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="F9" t="n">
         <v>2.0</v>
@@ -726,111 +876,87 @@
         <v>45.0</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s">
         <v>51</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="F12" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G12" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H12" t="n">
-        <v>36.0</v>
+        <v>60.0</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="F13" t="n">
         <v>1.0</v>
@@ -842,319 +968,319 @@
         <v>36.0</v>
       </c>
       <c r="I13" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="F14" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G14" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H14" t="n">
-        <v>45.0</v>
+        <v>36.0</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F15" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G15" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H15" t="n">
-        <v>45.0</v>
+        <v>36.0</v>
       </c>
       <c r="I15" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="F16" t="n">
         <v>2.0</v>
       </c>
       <c r="G16" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H16" t="n">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
       <c r="I16" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="F17" t="n">
         <v>2.0</v>
       </c>
       <c r="G17" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H17" t="n">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="F18" t="n">
         <v>2.0</v>
       </c>
       <c r="G18" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H18" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G19" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="H19" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" t="s">
         <v>51</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G20" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H20" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I20" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" t="s">
-        <v>25</v>
+        <v>67</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>45.0</v>
       </c>
       <c r="I22" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="I23" t="s">
         <v>56</v>
-      </c>
-      <c r="D23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G23" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H23" t="n">
-        <v>56.0</v>
-      </c>
-      <c r="I23" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F24" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G24" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H24" t="n">
-        <v>56.0</v>
+        <v>36.0</v>
       </c>
       <c r="I24" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="F25" t="n">
         <v>2.0</v>
@@ -1166,24 +1292,24 @@
         <v>56.0</v>
       </c>
       <c r="I25" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F26" t="n">
         <v>2.0</v>
@@ -1195,111 +1321,87 @@
         <v>56.0</v>
       </c>
       <c r="I26" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="F27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G27" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H27" t="n">
-        <v>36.0</v>
+        <v>56.0</v>
       </c>
       <c r="I27" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H28" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I28" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G29" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H29" t="n">
-        <v>45.0</v>
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" t="s">
+        <v>50</v>
       </c>
       <c r="I29" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="F30" t="n">
         <v>2.0</v>
@@ -1308,85 +1410,85 @@
         <v>3.0</v>
       </c>
       <c r="H30" t="n">
-        <v>45.0</v>
+        <v>56.0</v>
       </c>
       <c r="I30" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F31" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G31" t="n">
         <v>2.0</v>
       </c>
       <c r="H31" t="n">
-        <v>40.0</v>
+        <v>36.0</v>
       </c>
       <c r="I31" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F32" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G32" t="n">
         <v>2.0</v>
       </c>
       <c r="H32" t="n">
-        <v>40.0</v>
+        <v>36.0</v>
       </c>
       <c r="I32" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="F33" t="n">
         <v>2.0</v>
@@ -1398,169 +1500,145 @@
         <v>45.0</v>
       </c>
       <c r="I33" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F34" t="n">
         <v>2.0</v>
       </c>
       <c r="G34" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H34" t="n">
-        <v>60.0</v>
+        <v>45.0</v>
       </c>
       <c r="I34" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
         <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F35" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G35" t="n">
         <v>2.0</v>
       </c>
       <c r="H35" t="n">
-        <v>36.0</v>
+        <v>40.0</v>
       </c>
       <c r="I35" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="F36" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G36" t="n">
         <v>2.0</v>
       </c>
       <c r="H36" t="n">
-        <v>36.0</v>
+        <v>40.0</v>
       </c>
       <c r="I36" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G37" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H37" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I37" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E38" t="s">
-        <v>36</v>
-      </c>
-      <c r="F38" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G38" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H38" t="n">
-        <v>45.0</v>
+        <v>47</v>
+      </c>
+      <c r="F38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" t="s">
+        <v>50</v>
       </c>
       <c r="I38" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="E39" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="F39" t="n">
         <v>2.0</v>
@@ -1572,290 +1650,290 @@
         <v>45.0</v>
       </c>
       <c r="I39" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="D40" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="E40" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="F40" t="n">
         <v>2.0</v>
       </c>
       <c r="G40" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H40" t="n">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c r="I40" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E41" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="F41" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G41" t="n">
         <v>2.0</v>
       </c>
       <c r="H41" t="n">
-        <v>40.0</v>
+        <v>36.0</v>
       </c>
       <c r="I41" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E42" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F42" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G42" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H42" t="n">
-        <v>45.0</v>
+        <v>36.0</v>
       </c>
       <c r="I42" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D43" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E43" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F43" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G43" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H43" t="n">
-        <v>60.0</v>
+        <v>36.0</v>
       </c>
       <c r="I43" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D44" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="E44" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F44" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G44" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H44" t="n">
-        <v>36.0</v>
+        <v>45.0</v>
       </c>
       <c r="I44" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s">
+        <v>63</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" t="s">
-        <v>23</v>
-      </c>
-      <c r="G46" t="s">
-        <v>24</v>
-      </c>
-      <c r="H46" t="s">
-        <v>25</v>
-      </c>
-      <c r="I46" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="E47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" t="s">
+        <v>48</v>
+      </c>
+      <c r="G47" t="s">
+        <v>49</v>
+      </c>
+      <c r="H47" t="s">
+        <v>50</v>
+      </c>
+      <c r="I47" t="s">
         <v>51</v>
-      </c>
-      <c r="F47" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G47" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H47" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="I47" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="D48" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="E48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F48" t="n">
         <v>2.0</v>
       </c>
       <c r="G48" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H48" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="I48" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="E49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F49" t="n">
         <v>2.0</v>
       </c>
       <c r="G49" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H49" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="I49" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="D50" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="E50" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="F50" t="n">
         <v>2.0</v>
@@ -1864,85 +1942,85 @@
         <v>3.0</v>
       </c>
       <c r="H50" t="n">
-        <v>50.0</v>
+        <v>45.0</v>
       </c>
       <c r="I50" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" t="s">
+        <v>72</v>
+      </c>
+      <c r="F51" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="I51" t="s">
         <v>56</v>
-      </c>
-      <c r="D51" t="s">
-        <v>64</v>
-      </c>
-      <c r="E51" t="s">
-        <v>65</v>
-      </c>
-      <c r="F51" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G51" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H51" t="n">
-        <v>56.0</v>
-      </c>
-      <c r="I51" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E52" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F52" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G52" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H52" t="n">
-        <v>56.0</v>
+        <v>36.0</v>
       </c>
       <c r="I52" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E53" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F53" t="n">
         <v>2.0</v>
@@ -1951,27 +2029,27 @@
         <v>3.0</v>
       </c>
       <c r="H53" t="n">
-        <v>56.0</v>
+        <v>50.0</v>
       </c>
       <c r="I53" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
         <v>10</v>
       </c>
-      <c r="C54" t="s">
-        <v>59</v>
-      </c>
       <c r="D54" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E54" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F54" t="n">
         <v>2.0</v>
@@ -1980,68 +2058,44 @@
         <v>3.0</v>
       </c>
       <c r="H54" t="n">
-        <v>56.0</v>
+        <v>50.0</v>
       </c>
       <c r="I54" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" t="s">
-        <v>29</v>
-      </c>
-      <c r="E55" t="s">
-        <v>30</v>
-      </c>
-      <c r="F55" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H55" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I55" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D56" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
-      </c>
-      <c r="F56" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H56" t="n">
-        <v>36.0</v>
+        <v>47</v>
+      </c>
+      <c r="F56" t="s">
+        <v>48</v>
+      </c>
+      <c r="G56" t="s">
+        <v>49</v>
+      </c>
+      <c r="H56" t="s">
+        <v>50</v>
       </c>
       <c r="I56" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57">
@@ -2049,16 +2103,16 @@
         <v>105</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="E57" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="F57" t="n">
         <v>2.0</v>
@@ -2067,28 +2121,28 @@
         <v>3.0</v>
       </c>
       <c r="H57" t="n">
-        <v>45.0</v>
+        <v>50.0</v>
       </c>
       <c r="I57" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
+        <v>118</v>
+      </c>
+      <c r="E58" t="s">
         <v>63</v>
       </c>
-      <c r="D58" t="s">
-        <v>35</v>
-      </c>
-      <c r="E58" t="s">
-        <v>38</v>
-      </c>
       <c r="F58" t="n">
         <v>2.0</v>
       </c>
@@ -2096,85 +2150,85 @@
         <v>3.0</v>
       </c>
       <c r="H58" t="n">
-        <v>45.0</v>
+        <v>50.0</v>
       </c>
       <c r="I58" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D59" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="E59" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="F59" t="n">
         <v>2.0</v>
       </c>
       <c r="G59" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H59" t="n">
-        <v>40.0</v>
+        <v>56.0</v>
       </c>
       <c r="I59" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D60" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="E60" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="F60" t="n">
         <v>2.0</v>
       </c>
       <c r="G60" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H60" t="n">
-        <v>40.0</v>
+        <v>56.0</v>
       </c>
       <c r="I60" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D61" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="E61" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="F61" t="n">
         <v>2.0</v>
@@ -2183,56 +2237,56 @@
         <v>3.0</v>
       </c>
       <c r="H61" t="n">
-        <v>45.0</v>
+        <v>56.0</v>
       </c>
       <c r="I61" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D62" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="E62" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F62" t="n">
         <v>2.0</v>
       </c>
       <c r="G62" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H62" t="n">
-        <v>60.0</v>
+        <v>56.0</v>
       </c>
       <c r="I62" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D63" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E63" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F63" t="n">
         <v>1.0</v>
@@ -2244,111 +2298,87 @@
         <v>36.0</v>
       </c>
       <c r="I63" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>107</v>
-      </c>
-      <c r="B64" t="s">
-        <v>39</v>
-      </c>
-      <c r="C64" t="s">
-        <v>76</v>
-      </c>
-      <c r="D64" t="s">
-        <v>29</v>
-      </c>
-      <c r="E64" t="s">
-        <v>30</v>
-      </c>
-      <c r="F64" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G64" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H64" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I64" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="B65" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C65" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="D65" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E65" t="s">
-        <v>30</v>
-      </c>
-      <c r="F65" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G65" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H65" t="n">
-        <v>36.0</v>
+        <v>47</v>
+      </c>
+      <c r="F65" t="s">
+        <v>48</v>
+      </c>
+      <c r="G65" t="s">
+        <v>49</v>
+      </c>
+      <c r="H65" t="s">
+        <v>50</v>
       </c>
       <c r="I65" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C66" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D66" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="E66" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="F66" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G66" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H66" t="n">
-        <v>45.0</v>
+        <v>36.0</v>
       </c>
       <c r="I66" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="B67" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D67" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E67" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="F67" t="n">
         <v>2.0</v>
@@ -2360,53 +2390,53 @@
         <v>45.0</v>
       </c>
       <c r="I67" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B68" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D68" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E68" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="F68" t="n">
         <v>2.0</v>
       </c>
       <c r="G68" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H68" t="n">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
       <c r="I68" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B69" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C69" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D69" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E69" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="F69" t="n">
         <v>2.0</v>
@@ -2418,36 +2448,36 @@
         <v>40.0</v>
       </c>
       <c r="I69" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B70" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D70" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E70" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="F70" t="n">
         <v>2.0</v>
       </c>
       <c r="G70" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H70" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
       <c r="I70" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71">
@@ -2455,57 +2485,294 @@
         <v>114</v>
       </c>
       <c r="B71" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D71" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="E71" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="F71" t="n">
         <v>2.0</v>
       </c>
       <c r="G71" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H71" t="n">
-        <v>60.0</v>
+        <v>45.0</v>
       </c>
       <c r="I71" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B72" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C72" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D72" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="E72" t="s">
+        <v>72</v>
+      </c>
+      <c r="F72" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="I72" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" t="s">
+        <v>45</v>
+      </c>
+      <c r="D74" t="s">
+        <v>46</v>
+      </c>
+      <c r="E74" t="s">
+        <v>47</v>
+      </c>
+      <c r="F74" t="s">
+        <v>48</v>
+      </c>
+      <c r="G74" t="s">
+        <v>49</v>
+      </c>
+      <c r="H74" t="s">
+        <v>50</v>
+      </c>
+      <c r="I74" t="s">
         <v>51</v>
       </c>
-      <c r="F72" t="n">
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>125</v>
+      </c>
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" t="s">
+        <v>93</v>
+      </c>
+      <c r="D75" t="s">
+        <v>54</v>
+      </c>
+      <c r="E75" t="s">
+        <v>72</v>
+      </c>
+      <c r="F75" t="n">
         <v>1.0</v>
       </c>
-      <c r="G72" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H72" t="n">
+      <c r="G75" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H75" t="n">
         <v>36.0</v>
       </c>
-      <c r="I72" t="s">
-        <v>31</v>
+      <c r="I75" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>126</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E76" t="s">
+        <v>55</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="I76" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>127</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" t="s">
+        <v>99</v>
+      </c>
+      <c r="D77" t="s">
+        <v>54</v>
+      </c>
+      <c r="E77" t="s">
+        <v>55</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H77" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="I77" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>128</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" t="s">
+        <v>101</v>
+      </c>
+      <c r="D78" t="s">
+        <v>60</v>
+      </c>
+      <c r="E78" t="s">
+        <v>61</v>
+      </c>
+      <c r="F78" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H78" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="I78" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>129</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" t="s">
+        <v>109</v>
+      </c>
+      <c r="D79" t="s">
+        <v>60</v>
+      </c>
+      <c r="E79" t="s">
+        <v>63</v>
+      </c>
+      <c r="F79" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H79" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="I79" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>130</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80" t="s">
+        <v>65</v>
+      </c>
+      <c r="E80" t="s">
+        <v>63</v>
+      </c>
+      <c r="F80" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H80" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="I80" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" t="s">
+        <v>119</v>
+      </c>
+      <c r="D81" t="s">
+        <v>65</v>
+      </c>
+      <c r="E81" t="s">
+        <v>67</v>
+      </c>
+      <c r="F81" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H81" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparando EP4, Abstraccion mejorada, y herencia todo funciona, se implementara interfaces en el siguiente commit
</commit_message>
<xml_diff>
--- a/Reporte_Gestion_Inmobiliaria.xlsx
+++ b/Reporte_Gestion_Inmobiliaria.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="132">
   <si>
     <t>Id Edificio</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Metro cuadrados</t>
   </si>
   <si>
-    <t>Disponibilidad departamento</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -183,15 +180,9 @@
     <t>Sur</t>
   </si>
   <si>
-    <t>Disponible</t>
-  </si>
-  <si>
     <t>120</t>
   </si>
   <si>
-    <t>vendido</t>
-  </si>
-  <si>
     <t>130</t>
   </si>
   <si>
@@ -300,30 +291,30 @@
     <t>26</t>
   </si>
   <si>
+    <t>27</t>
+  </si>
+  <si>
     <t>31</t>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>32</t>
   </si>
   <si>
-    <t>28</t>
+    <t>29</t>
   </si>
   <si>
     <t>33</t>
   </si>
   <si>
-    <t>29</t>
+    <t>30</t>
   </si>
   <si>
     <t>34</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>35</t>
   </si>
   <si>
@@ -339,36 +330,36 @@
     <t>44</t>
   </si>
   <si>
+    <t>36</t>
+  </si>
+  <si>
     <t>51</t>
   </si>
   <si>
-    <t>36</t>
+    <t>37</t>
   </si>
   <si>
     <t>52</t>
   </si>
   <si>
-    <t>37</t>
+    <t>38</t>
   </si>
   <si>
     <t>53</t>
   </si>
   <si>
-    <t>38</t>
+    <t>39</t>
   </si>
   <si>
     <t>54</t>
   </si>
   <si>
-    <t>39</t>
+    <t>40</t>
   </si>
   <si>
     <t>55</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>3420</t>
   </si>
   <si>
@@ -393,6 +384,12 @@
     <t>56</t>
   </si>
   <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>24590</t>
+  </si>
+  <si>
     <t>57</t>
   </si>
   <si>
@@ -409,6 +406,9 @@
   </si>
   <si>
     <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
   </si>
 </sst>
 </file>
@@ -636,7 +636,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -672,25 +672,22 @@
       <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>54</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
       </c>
       <c r="F3" t="n">
         <v>1.0</v>
@@ -700,9 +697,6 @@
       </c>
       <c r="H3" t="n">
         <v>36.0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4">
@@ -713,13 +707,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
         <v>54</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
       </c>
       <c r="F4" t="n">
         <v>1.0</v>
@@ -729,9 +723,6 @@
       </c>
       <c r="H4" t="n">
         <v>36.0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5">
@@ -742,13 +733,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F5" t="n">
         <v>2.0</v>
@@ -758,9 +749,6 @@
       </c>
       <c r="H5" t="n">
         <v>45.0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6">
@@ -771,13 +759,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
         <v>60</v>
-      </c>
-      <c r="E6" t="s">
-        <v>63</v>
       </c>
       <c r="F6" t="n">
         <v>2.0</v>
@@ -787,9 +775,6 @@
       </c>
       <c r="H6" t="n">
         <v>45.0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7">
@@ -800,13 +785,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F7" t="n">
         <v>2.0</v>
@@ -816,9 +801,6 @@
       </c>
       <c r="H7" t="n">
         <v>40.0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8">
@@ -829,13 +811,13 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F8" t="n">
         <v>2.0</v>
@@ -845,9 +827,6 @@
       </c>
       <c r="H8" t="n">
         <v>40.0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9">
@@ -858,13 +837,13 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F9" t="n">
         <v>2.0</v>
@@ -874,9 +853,6 @@
       </c>
       <c r="H9" t="n">
         <v>45.0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10">
@@ -909,9 +885,6 @@
       <c r="H11" t="s">
         <v>50</v>
       </c>
-      <c r="I11" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -921,13 +894,13 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F12" t="n">
         <v>2.0</v>
@@ -937,9 +910,6 @@
       </c>
       <c r="H12" t="n">
         <v>60.0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -950,13 +920,13 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F13" t="n">
         <v>1.0</v>
@@ -966,9 +936,6 @@
       </c>
       <c r="H13" t="n">
         <v>36.0</v>
-      </c>
-      <c r="I13" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -979,13 +946,13 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
       </c>
       <c r="F14" t="n">
         <v>1.0</v>
@@ -996,25 +963,22 @@
       <c r="H14" t="n">
         <v>36.0</v>
       </c>
-      <c r="I14" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
         <v>54</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
       </c>
       <c r="F15" t="n">
         <v>1.0</v>
@@ -1025,25 +989,22 @@
       <c r="H15" t="n">
         <v>36.0</v>
       </c>
-      <c r="I15" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F16" t="n">
         <v>2.0</v>
@@ -1054,25 +1015,22 @@
       <c r="H16" t="n">
         <v>45.0</v>
       </c>
-      <c r="I16" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="s">
         <v>60</v>
-      </c>
-      <c r="E17" t="s">
-        <v>63</v>
       </c>
       <c r="F17" t="n">
         <v>2.0</v>
@@ -1083,25 +1041,22 @@
       <c r="H17" t="n">
         <v>45.0</v>
       </c>
-      <c r="I17" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F18" t="n">
         <v>2.0</v>
@@ -1111,9 +1066,6 @@
       </c>
       <c r="H18" t="n">
         <v>40.0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19">
@@ -1146,25 +1098,22 @@
       <c r="H20" t="s">
         <v>50</v>
       </c>
-      <c r="I20" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F21" t="n">
         <v>2.0</v>
@@ -1175,25 +1124,22 @@
       <c r="H21" t="n">
         <v>40.0</v>
       </c>
-      <c r="I21" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F22" t="n">
         <v>2.0</v>
@@ -1204,25 +1150,22 @@
       <c r="H22" t="n">
         <v>45.0</v>
       </c>
-      <c r="I22" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F23" t="n">
         <v>2.0</v>
@@ -1233,25 +1176,22 @@
       <c r="H23" t="n">
         <v>60.0</v>
       </c>
-      <c r="I23" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F24" t="n">
         <v>1.0</v>
@@ -1262,25 +1202,22 @@
       <c r="H24" t="n">
         <v>36.0</v>
       </c>
-      <c r="I24" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F25" t="n">
         <v>2.0</v>
@@ -1291,25 +1228,22 @@
       <c r="H25" t="n">
         <v>56.0</v>
       </c>
-      <c r="I25" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
         <v>83</v>
-      </c>
-      <c r="E26" t="s">
-        <v>86</v>
       </c>
       <c r="F26" t="n">
         <v>2.0</v>
@@ -1320,25 +1254,22 @@
       <c r="H26" t="n">
         <v>56.0</v>
       </c>
-      <c r="I26" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F27" t="n">
         <v>2.0</v>
@@ -1349,117 +1280,105 @@
       <c r="H27" t="n">
         <v>56.0</v>
       </c>
-      <c r="I27" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>56.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" t="s">
-        <v>48</v>
-      </c>
-      <c r="G29" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G30" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H30" t="n">
-        <v>56.0</v>
-      </c>
-      <c r="I30" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F31" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G31" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H31" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I31" t="s">
-        <v>56</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
         <v>54</v>
-      </c>
-      <c r="E32" t="s">
-        <v>55</v>
       </c>
       <c r="F32" t="n">
         <v>1.0</v>
@@ -1470,54 +1389,48 @@
       <c r="H32" t="n">
         <v>36.0</v>
       </c>
-      <c r="I32" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F33" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G33" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H33" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="I33" t="s">
-        <v>58</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F34" t="n">
         <v>2.0</v>
@@ -1528,54 +1441,48 @@
       <c r="H34" t="n">
         <v>45.0</v>
       </c>
-      <c r="I34" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F35" t="n">
         <v>2.0</v>
       </c>
       <c r="G35" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H35" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="I35" t="s">
-        <v>58</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B36" t="s">
         <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F36" t="n">
         <v>2.0</v>
@@ -1586,146 +1493,131 @@
       <c r="H36" t="n">
         <v>40.0</v>
       </c>
-      <c r="I36" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>94</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>40.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" t="s">
-        <v>47</v>
-      </c>
-      <c r="F38" t="s">
-        <v>48</v>
-      </c>
-      <c r="G38" t="s">
-        <v>49</v>
-      </c>
-      <c r="H38" t="s">
-        <v>50</v>
-      </c>
-      <c r="I38" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="E39" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G39" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H39" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="I39" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="F39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E40" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F40" t="n">
         <v>2.0</v>
       </c>
       <c r="G40" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H40" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="I40" t="s">
-        <v>56</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E41" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F41" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G41" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H41" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I41" t="s">
-        <v>56</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F42" t="n">
         <v>1.0</v>
@@ -1736,25 +1628,22 @@
       <c r="H42" t="n">
         <v>36.0</v>
       </c>
-      <c r="I42" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
         <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" t="s">
         <v>54</v>
-      </c>
-      <c r="E43" t="s">
-        <v>55</v>
       </c>
       <c r="F43" t="n">
         <v>1.0</v>
@@ -1765,54 +1654,48 @@
       <c r="H43" t="n">
         <v>36.0</v>
       </c>
-      <c r="I43" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s">
         <v>18</v>
       </c>
       <c r="C44" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F44" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G44" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H44" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="I44" t="s">
-        <v>58</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F45" t="n">
         <v>2.0</v>
@@ -1823,88 +1706,79 @@
       <c r="H45" t="n">
         <v>45.0</v>
       </c>
-      <c r="I45" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>45.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" t="s">
-        <v>46</v>
-      </c>
-      <c r="E47" t="s">
-        <v>47</v>
-      </c>
-      <c r="F47" t="s">
-        <v>48</v>
-      </c>
-      <c r="G47" t="s">
-        <v>49</v>
-      </c>
-      <c r="H47" t="s">
-        <v>50</v>
-      </c>
-      <c r="I47" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="E48" t="s">
-        <v>63</v>
-      </c>
-      <c r="F48" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H48" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="I48" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="F48" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48" t="s">
+        <v>49</v>
+      </c>
+      <c r="H48" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C49" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D49" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E49" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F49" t="n">
         <v>2.0</v>
@@ -1915,141 +1789,126 @@
       <c r="H49" t="n">
         <v>40.0</v>
       </c>
-      <c r="I49" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
         <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D50" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E50" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F50" t="n">
         <v>2.0</v>
       </c>
       <c r="G50" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H50" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="I50" t="s">
-        <v>58</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B51" t="s">
         <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D51" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E51" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F51" t="n">
         <v>2.0</v>
       </c>
       <c r="G51" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H51" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="I51" t="s">
-        <v>56</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E52" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F52" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G52" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H52" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I52" t="s">
-        <v>56</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>5</v>
+        <v>114</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="E53" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F53" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G53" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H53" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="I53" t="s">
-        <v>58</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E54" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F54" t="n">
         <v>2.0</v>
@@ -2060,88 +1919,79 @@
       <c r="H54" t="n">
         <v>50.0</v>
       </c>
-      <c r="I54" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>102</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>43</v>
-      </c>
-      <c r="B56" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" t="s">
-        <v>45</v>
-      </c>
-      <c r="D56" t="s">
-        <v>46</v>
-      </c>
-      <c r="E56" t="s">
-        <v>47</v>
-      </c>
-      <c r="F56" t="s">
-        <v>48</v>
-      </c>
-      <c r="G56" t="s">
-        <v>49</v>
-      </c>
-      <c r="H56" t="s">
-        <v>50</v>
-      </c>
-      <c r="I56" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D57" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="E57" t="s">
-        <v>88</v>
-      </c>
-      <c r="F57" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G57" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H57" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="I57" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="F57" t="s">
+        <v>48</v>
+      </c>
+      <c r="G57" t="s">
+        <v>49</v>
+      </c>
+      <c r="H57" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B58" t="s">
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E58" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="F58" t="n">
         <v>2.0</v>
@@ -2152,25 +2002,22 @@
       <c r="H58" t="n">
         <v>50.0</v>
       </c>
-      <c r="I58" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="E59" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="F59" t="n">
         <v>2.0</v>
@@ -2179,27 +2026,24 @@
         <v>3.0</v>
       </c>
       <c r="H59" t="n">
-        <v>56.0</v>
-      </c>
-      <c r="I59" t="s">
-        <v>58</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D60" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E60" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F60" t="n">
         <v>2.0</v>
@@ -2210,25 +2054,22 @@
       <c r="H60" t="n">
         <v>56.0</v>
       </c>
-      <c r="I60" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D61" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" t="s">
         <v>83</v>
-      </c>
-      <c r="E61" t="s">
-        <v>88</v>
       </c>
       <c r="F61" t="n">
         <v>2.0</v>
@@ -2239,25 +2080,22 @@
       <c r="H61" t="n">
         <v>56.0</v>
       </c>
-      <c r="I61" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D62" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="F62" t="n">
         <v>2.0</v>
@@ -2268,146 +2106,131 @@
       <c r="H62" t="n">
         <v>56.0</v>
       </c>
-      <c r="I62" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D63" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="E63" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F63" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G63" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H63" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I63" t="s">
-        <v>56</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>120</v>
+      </c>
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" t="s">
+        <v>53</v>
+      </c>
+      <c r="E64" t="s">
+        <v>54</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>36.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>43</v>
-      </c>
-      <c r="B65" t="s">
-        <v>44</v>
-      </c>
-      <c r="C65" t="s">
-        <v>45</v>
-      </c>
-      <c r="D65" t="s">
-        <v>46</v>
-      </c>
-      <c r="E65" t="s">
-        <v>47</v>
-      </c>
-      <c r="F65" t="s">
-        <v>48</v>
-      </c>
-      <c r="G65" t="s">
-        <v>49</v>
-      </c>
-      <c r="H65" t="s">
-        <v>50</v>
-      </c>
-      <c r="I65" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>43</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="D66" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E66" t="s">
-        <v>55</v>
-      </c>
-      <c r="F66" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G66" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H66" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I66" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="F66" t="s">
+        <v>48</v>
+      </c>
+      <c r="G66" t="s">
+        <v>49</v>
+      </c>
+      <c r="H66" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D67" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E67" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F67" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G67" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H67" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="I67" t="s">
-        <v>58</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D68" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E68" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F68" t="n">
         <v>2.0</v>
@@ -2418,54 +2241,48 @@
       <c r="H68" t="n">
         <v>45.0</v>
       </c>
-      <c r="I68" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D69" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E69" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F69" t="n">
         <v>2.0</v>
       </c>
       <c r="G69" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H69" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="I69" t="s">
-        <v>58</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B70" t="s">
         <v>14</v>
       </c>
       <c r="C70" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D70" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E70" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F70" t="n">
         <v>2.0</v>
@@ -2476,175 +2293,157 @@
       <c r="H70" t="n">
         <v>40.0</v>
       </c>
-      <c r="I70" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B71" t="s">
         <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D71" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E71" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F71" t="n">
         <v>2.0</v>
       </c>
       <c r="G71" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H71" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="I71" t="s">
-        <v>58</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
         <v>14</v>
       </c>
       <c r="C72" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D72" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E72" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F72" t="n">
         <v>2.0</v>
       </c>
       <c r="G72" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H72" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="I72" t="s">
-        <v>56</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>122</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" t="s">
+        <v>89</v>
+      </c>
+      <c r="D73" t="s">
+        <v>68</v>
+      </c>
+      <c r="E73" t="s">
+        <v>69</v>
+      </c>
+      <c r="F73" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>60.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
       <c r="B74" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="D74" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="E74" t="s">
-        <v>47</v>
-      </c>
-      <c r="F74" t="s">
-        <v>48</v>
-      </c>
-      <c r="G74" t="s">
-        <v>49</v>
-      </c>
-      <c r="H74" t="s">
-        <v>50</v>
-      </c>
-      <c r="I74" t="s">
-        <v>51</v>
+        <v>58</v>
+      </c>
+      <c r="F74" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>30.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>125</v>
-      </c>
-      <c r="B75" t="s">
-        <v>14</v>
-      </c>
-      <c r="C75" t="s">
-        <v>93</v>
-      </c>
-      <c r="D75" t="s">
-        <v>54</v>
-      </c>
-      <c r="E75" t="s">
-        <v>72</v>
-      </c>
-      <c r="F75" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G75" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H75" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I75" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>126</v>
+        <v>43</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="D76" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E76" t="s">
-        <v>55</v>
-      </c>
-      <c r="F76" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G76" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H76" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="I76" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="F76" t="s">
+        <v>48</v>
+      </c>
+      <c r="G76" t="s">
+        <v>49</v>
+      </c>
+      <c r="H76" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B77" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C77" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E77" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F77" t="n">
         <v>1.0</v>
@@ -2655,124 +2454,161 @@
       <c r="H77" t="n">
         <v>36.0</v>
       </c>
-      <c r="I77" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B78" t="s">
         <v>18</v>
       </c>
       <c r="C78" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D78" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E78" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F78" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G78" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H78" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="I78" t="s">
-        <v>58</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D79" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E79" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F79" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G79" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H79" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="I79" t="s">
-        <v>56</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B80" t="s">
         <v>18</v>
       </c>
       <c r="C80" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D80" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E80" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F80" t="n">
         <v>2.0</v>
       </c>
       <c r="G80" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H80" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="I80" t="s">
-        <v>58</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" t="s">
+        <v>105</v>
+      </c>
+      <c r="D81" t="s">
+        <v>57</v>
+      </c>
+      <c r="E81" t="s">
+        <v>60</v>
+      </c>
+      <c r="F81" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H81" t="n">
+        <v>45.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" t="s">
+        <v>107</v>
+      </c>
+      <c r="D82" t="s">
+        <v>62</v>
+      </c>
+      <c r="E82" t="s">
+        <v>60</v>
+      </c>
+      <c r="F82" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H82" t="n">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
         <v>131</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B83" t="s">
         <v>22</v>
       </c>
-      <c r="C81" t="s">
-        <v>119</v>
-      </c>
-      <c r="D81" t="s">
-        <v>65</v>
-      </c>
-      <c r="E81" t="s">
-        <v>67</v>
-      </c>
-      <c r="F81" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G81" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H81" t="n">
+      <c r="C83" t="s">
+        <v>116</v>
+      </c>
+      <c r="D83" t="s">
+        <v>62</v>
+      </c>
+      <c r="E83" t="s">
+        <v>64</v>
+      </c>
+      <c r="F83" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H83" t="n">
         <v>40.0</v>
-      </c>
-      <c r="I81" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparando EP4, Se agrego interface en clase Departamento para crear y mostrar informes de disponibilidad en el menú, opción 11.
</commit_message>
<xml_diff>
--- a/Reporte_Gestion_Inmobiliaria.xlsx
+++ b/Reporte_Gestion_Inmobiliaria.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="129">
   <si>
     <t>Id Edificio</t>
   </si>
@@ -291,30 +291,30 @@
     <t>26</t>
   </si>
   <si>
+    <t>31</t>
+  </si>
+  <si>
     <t>27</t>
   </si>
   <si>
-    <t>31</t>
+    <t>32</t>
   </si>
   <si>
     <t>28</t>
   </si>
   <si>
-    <t>32</t>
+    <t>33</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>33</t>
+    <t>34</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
     <t>35</t>
   </si>
   <si>
@@ -330,36 +330,36 @@
     <t>44</t>
   </si>
   <si>
+    <t>51</t>
+  </si>
+  <si>
     <t>36</t>
   </si>
   <si>
-    <t>51</t>
+    <t>52</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>52</t>
+    <t>53</t>
   </si>
   <si>
     <t>38</t>
   </si>
   <si>
-    <t>53</t>
+    <t>54</t>
   </si>
   <si>
     <t>39</t>
   </si>
   <si>
-    <t>54</t>
+    <t>55</t>
   </si>
   <si>
     <t>40</t>
   </si>
   <si>
-    <t>55</t>
-  </si>
-  <si>
     <t>3420</t>
   </si>
   <si>
@@ -384,12 +384,6 @@
     <t>56</t>
   </si>
   <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>24590</t>
-  </si>
-  <si>
     <t>57</t>
   </si>
   <si>
@@ -406,9 +400,6 @@
   </si>
   <si>
     <t>62</t>
-  </si>
-  <si>
-    <t>63</t>
   </si>
 </sst>
 </file>
@@ -636,7 +627,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1283,59 +1274,59 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H28" t="n">
-        <v>56.0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" t="s">
-        <v>48</v>
-      </c>
-      <c r="G30" t="s">
-        <v>49</v>
-      </c>
-      <c r="H30" t="s">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>56.0</v>
       </c>
     </row>
     <row r="31">
@@ -1343,25 +1334,25 @@
         <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F31" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G31" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H31" t="n">
-        <v>56.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="32">
@@ -1372,7 +1363,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
         <v>53</v>
@@ -1398,22 +1389,22 @@
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F33" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G33" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H33" t="n">
-        <v>36.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="34">
@@ -1424,13 +1415,13 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D34" t="s">
         <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F34" t="n">
         <v>2.0</v>
@@ -1447,13 +1438,13 @@
         <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E35" t="s">
         <v>60</v>
@@ -1462,27 +1453,27 @@
         <v>2.0</v>
       </c>
       <c r="G35" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H35" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
         <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D36" t="s">
         <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F36" t="n">
         <v>2.0</v>
@@ -1496,128 +1487,128 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>94</v>
-      </c>
-      <c r="B37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>95</v>
-      </c>
-      <c r="D37" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G37" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H37" t="n">
-        <v>40.0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="E39" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" t="s">
-        <v>48</v>
-      </c>
-      <c r="G39" t="s">
-        <v>49</v>
-      </c>
-      <c r="H39" t="s">
-        <v>50</v>
+        <v>64</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>45.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E40" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F40" t="n">
         <v>2.0</v>
       </c>
       <c r="G40" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H40" t="n">
-        <v>45.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
         <v>69</v>
       </c>
       <c r="F41" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G41" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H41" t="n">
-        <v>60.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F42" t="n">
         <v>1.0</v>
@@ -1631,13 +1622,13 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
         <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
         <v>53</v>
@@ -1657,45 +1648,45 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
         <v>18</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D44" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E44" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F44" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G44" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H44" t="n">
-        <v>36.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B45" t="s">
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D45" t="s">
         <v>57</v>
       </c>
       <c r="E45" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F45" t="n">
         <v>2.0</v>
@@ -1709,76 +1700,76 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" t="s">
-        <v>57</v>
-      </c>
-      <c r="E46" t="s">
-        <v>60</v>
-      </c>
-      <c r="F46" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H46" t="n">
-        <v>45.0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>43</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" t="s">
+        <v>48</v>
+      </c>
+      <c r="G47" t="s">
+        <v>49</v>
+      </c>
+      <c r="H47" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="D48" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="E48" t="s">
-        <v>47</v>
-      </c>
-      <c r="F48" t="s">
-        <v>48</v>
-      </c>
-      <c r="G48" t="s">
-        <v>49</v>
-      </c>
-      <c r="H48" t="s">
-        <v>50</v>
+        <v>60</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>40.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D49" t="s">
         <v>62</v>
       </c>
       <c r="E49" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F49" t="n">
         <v>2.0</v>
@@ -1792,16 +1783,16 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
         <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E50" t="s">
         <v>64</v>
@@ -1810,88 +1801,88 @@
         <v>2.0</v>
       </c>
       <c r="G50" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H50" t="n">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B51" t="s">
         <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E51" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F51" t="n">
         <v>2.0</v>
       </c>
       <c r="G51" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H51" t="n">
-        <v>45.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D52" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E52" t="s">
         <v>69</v>
       </c>
       <c r="F52" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G52" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H52" t="n">
-        <v>60.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="E53" t="s">
         <v>69</v>
       </c>
       <c r="F53" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G53" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H53" t="n">
-        <v>36.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="54">
@@ -1902,13 +1893,13 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D54" t="s">
         <v>115</v>
       </c>
       <c r="E54" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F54" t="n">
         <v>2.0</v>
@@ -1922,59 +1913,59 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" t="s">
-        <v>115</v>
-      </c>
-      <c r="E55" t="s">
-        <v>83</v>
-      </c>
-      <c r="F55" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H55" t="n">
-        <v>50.0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="B56" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D56" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" t="s">
+        <v>47</v>
+      </c>
+      <c r="F56" t="s">
+        <v>48</v>
+      </c>
+      <c r="G56" t="s">
+        <v>49</v>
+      </c>
+      <c r="H56" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="E57" t="s">
-        <v>47</v>
-      </c>
-      <c r="F57" t="s">
-        <v>48</v>
-      </c>
-      <c r="G57" t="s">
-        <v>49</v>
-      </c>
-      <c r="H57" t="s">
-        <v>50</v>
+        <v>85</v>
+      </c>
+      <c r="F57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="58">
@@ -1985,13 +1976,13 @@
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D58" t="s">
         <v>115</v>
       </c>
       <c r="E58" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="F58" t="n">
         <v>2.0</v>
@@ -2011,13 +2002,13 @@
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="D59" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E59" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="F59" t="n">
         <v>2.0</v>
@@ -2026,7 +2017,7 @@
         <v>3.0</v>
       </c>
       <c r="H59" t="n">
-        <v>50.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="60">
@@ -2037,13 +2028,13 @@
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D60" t="s">
         <v>80</v>
       </c>
       <c r="E60" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F60" t="n">
         <v>2.0</v>
@@ -2060,16 +2051,16 @@
         <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D61" t="s">
         <v>80</v>
       </c>
       <c r="E61" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F61" t="n">
         <v>2.0</v>
@@ -2089,13 +2080,13 @@
         <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D62" t="s">
         <v>80</v>
       </c>
       <c r="E62" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="F62" t="n">
         <v>2.0</v>
@@ -2115,79 +2106,79 @@
         <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D63" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="E63" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F63" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G63" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H63" t="n">
-        <v>56.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>120</v>
-      </c>
-      <c r="B64" t="s">
-        <v>10</v>
-      </c>
-      <c r="C64" t="s">
-        <v>76</v>
-      </c>
-      <c r="D64" t="s">
-        <v>53</v>
-      </c>
-      <c r="E64" t="s">
-        <v>54</v>
-      </c>
-      <c r="F64" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G64" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H64" t="n">
-        <v>36.0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="B65" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" t="s">
+        <v>46</v>
+      </c>
+      <c r="E65" t="s">
+        <v>47</v>
+      </c>
+      <c r="F65" t="s">
+        <v>48</v>
+      </c>
+      <c r="G65" t="s">
+        <v>49</v>
+      </c>
+      <c r="H65" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D66" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E66" t="s">
-        <v>47</v>
-      </c>
-      <c r="F66" t="s">
-        <v>48</v>
-      </c>
-      <c r="G66" t="s">
-        <v>49</v>
-      </c>
-      <c r="H66" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="F66" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>36.0</v>
       </c>
     </row>
     <row r="67">
@@ -2198,39 +2189,39 @@
         <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D67" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E67" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F67" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G67" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H67" t="n">
-        <v>36.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D68" t="s">
         <v>57</v>
       </c>
       <c r="E68" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F68" t="n">
         <v>2.0</v>
@@ -2244,16 +2235,16 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C69" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D69" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E69" t="s">
         <v>60</v>
@@ -2262,27 +2253,27 @@
         <v>2.0</v>
       </c>
       <c r="G69" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H69" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B70" t="s">
         <v>14</v>
       </c>
       <c r="C70" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D70" t="s">
         <v>62</v>
       </c>
       <c r="E70" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F70" t="n">
         <v>2.0</v>
@@ -2296,16 +2287,16 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B71" t="s">
         <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D71" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E71" t="s">
         <v>64</v>
@@ -2314,136 +2305,136 @@
         <v>2.0</v>
       </c>
       <c r="G71" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H71" t="n">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B72" t="s">
         <v>14</v>
       </c>
       <c r="C72" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D72" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E72" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F72" t="n">
         <v>2.0</v>
       </c>
       <c r="G72" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H72" t="n">
-        <v>45.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>122</v>
-      </c>
-      <c r="B73" t="s">
-        <v>14</v>
-      </c>
-      <c r="C73" t="s">
-        <v>89</v>
-      </c>
-      <c r="D73" t="s">
-        <v>68</v>
-      </c>
-      <c r="E73" t="s">
-        <v>69</v>
-      </c>
-      <c r="F73" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G73" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="H73" t="n">
-        <v>60.0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>123</v>
+        <v>43</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C74" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="D74" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="E74" t="s">
-        <v>58</v>
-      </c>
-      <c r="F74" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G74" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="H74" t="n">
-        <v>30.0</v>
+        <v>47</v>
+      </c>
+      <c r="F74" t="s">
+        <v>48</v>
+      </c>
+      <c r="G74" t="s">
+        <v>49</v>
+      </c>
+      <c r="H74" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>122</v>
+      </c>
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" t="s">
+        <v>90</v>
+      </c>
+      <c r="D75" t="s">
+        <v>53</v>
+      </c>
+      <c r="E75" t="s">
+        <v>69</v>
+      </c>
+      <c r="F75" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H75" t="n">
+        <v>36.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
       <c r="B76" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C76" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="D76" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E76" t="s">
-        <v>47</v>
-      </c>
-      <c r="F76" t="s">
-        <v>48</v>
-      </c>
-      <c r="G76" t="s">
-        <v>49</v>
-      </c>
-      <c r="H76" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>36.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B77" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C77" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D77" t="s">
         <v>53</v>
       </c>
       <c r="E77" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F77" t="n">
         <v>1.0</v>
@@ -2457,157 +2448,105 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B78" t="s">
         <v>18</v>
       </c>
       <c r="C78" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D78" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E78" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F78" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G78" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H78" t="n">
-        <v>36.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D79" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E79" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F79" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G79" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H79" t="n">
-        <v>36.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B80" t="s">
         <v>18</v>
       </c>
       <c r="C80" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D80" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E80" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F80" t="n">
         <v>2.0</v>
       </c>
       <c r="G80" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H80" t="n">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B81" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D81" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E81" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F81" t="n">
         <v>2.0</v>
       </c>
       <c r="G81" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H81" t="n">
-        <v>45.0</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s">
-        <v>130</v>
-      </c>
-      <c r="B82" t="s">
-        <v>18</v>
-      </c>
-      <c r="C82" t="s">
-        <v>107</v>
-      </c>
-      <c r="D82" t="s">
-        <v>62</v>
-      </c>
-      <c r="E82" t="s">
-        <v>60</v>
-      </c>
-      <c r="F82" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G82" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H82" t="n">
-        <v>40.0</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s">
-        <v>131</v>
-      </c>
-      <c r="B83" t="s">
-        <v>22</v>
-      </c>
-      <c r="C83" t="s">
-        <v>116</v>
-      </c>
-      <c r="D83" t="s">
-        <v>62</v>
-      </c>
-      <c r="E83" t="s">
-        <v>64</v>
-      </c>
-      <c r="F83" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G83" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H83" t="n">
         <v>40.0</v>
       </c>
     </row>

</xml_diff>